<commit_message>
Revert content to match upstream main
</commit_message>
<xml_diff>
--- a/dak-immz/IMMZ DAK_functional and non-functional requirements.xlsx
+++ b/dak-immz/IMMZ DAK_functional and non-functional requirements.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldhealthorg.sharepoint.com/sites/DigitalAcceleratorKits/Shared Documents/Immunizations Digital Accelerator Kit/_FINAL spreadsheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WHO\GitHub\smart-dak-immunizations\input\system-requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="46" documentId="8_{C37C3606-DD54-425E-9E4C-762F66653A6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{64052961-192B-4322-93FE-A2166E58DC74}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD41957E-10F4-49AF-98F7-8D47AB528321}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{D99AAAA5-616A-46C3-AA21-7263727BF10F}"/>
   </bookViews>
@@ -2314,7 +2314,7 @@
     <t>Be able to accommodate at least [x number of] concurrent users</t>
   </si>
   <si>
-    <t>https://smart.who.int/dak-immz/v1.0.0/IMMZ DAK_functional and non-functional requirements.xlsx
+    <t>https://smart.who.int/dak-immz/v0.9.9/IMMZ DAK_functional and non-functional requirements.xlsx
 © World Health Organization 2024. Some rights reserved. This work is available under the</t>
   </si>
 </sst>

</xml_diff>

<commit_message>
Import content from smart-dak-immz - gh-pages: sitepreview\dak-immz to folder dak-immz
</commit_message>
<xml_diff>
--- a/dak-immz/IMMZ DAK_functional and non-functional requirements.xlsx
+++ b/dak-immz/IMMZ DAK_functional and non-functional requirements.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WHO\GitHub\smart-dak-immunizations\input\system-requirements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldhealthorg.sharepoint.com/sites/DigitalAcceleratorKits/Shared Documents/Immunizations Digital Accelerator Kit/_FINAL spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD41957E-10F4-49AF-98F7-8D47AB528321}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="8_{C37C3606-DD54-425E-9E4C-762F66653A6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{64052961-192B-4322-93FE-A2166E58DC74}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{D99AAAA5-616A-46C3-AA21-7263727BF10F}"/>
   </bookViews>
@@ -2314,7 +2314,7 @@
     <t>Be able to accommodate at least [x number of] concurrent users</t>
   </si>
   <si>
-    <t>https://smart.who.int/dak-immz/v0.9.9/IMMZ DAK_functional and non-functional requirements.xlsx
+    <t>https://smart.who.int/dak-immz/v1.0.0/IMMZ DAK_functional and non-functional requirements.xlsx
 © World Health Organization 2024. Some rights reserved. This work is available under the</t>
   </si>
 </sst>

</xml_diff>